<commit_message>
Update library imports and enhance requirements
- Modified import statements in `pipeline.py` and `prompts.py` to reflect new module structure.
- Updated `requirements.txt` to include core dependencies and optional libraries for PDF processing and development/testing tools.
</commit_message>
<xml_diff>
--- a/pdfs/failed_ocr_pdfs.xlsx
+++ b/pdfs/failed_ocr_pdfs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,258 +433,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>_cleaned_A two-fold interpenetration pillar-layered metal-organic frameworks based on BODIPY for chemo-photodynamic therapy.pdf</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>_cleaned_A versatile and multifunctional metal-organic framework nanocomposite toward chemo-photodynamic therapy.pdf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>_cleaned_An insight into advanced approaches for photosensitizer optimization in endodontics—a critical review.pdf</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>_cleaned_Anthraquinone-Based Metal-Organic Frameworks as a Bifunctional Photocatalyst for C-H Activation.pdf</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>_cleaned_Antimicrobial photodynamic therapy assessment of three indocyanine green-loaded metal-organic frameworks against Enterococcus faecalis.pdf</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>_cleaned_Biomimetic Metal–Organic Framework Nanoparticles for Cooperative Combination of Antiangiogenesis and Photodynamic Therapy for Enhanced Efficacy.pdf</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>_cleaned_Boosting the photocatalytic CO2 reduction of metal-organic frameworks by encapsulating carbon dots.pdf</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>_cleaned_Boronic Acid-Decorated Multivariate Photosensitive Metal−Organic Frameworks for Combating Multi-Drug-Resistant Bacteria.pdf</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>_cleaned_Bromine Vapor Induced Continuous p- to n-Type Conversion of a Semiconductive Metal-Organic Framework Cu[Cu(pdt)2].pdf</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>_cleaned_Building a Pyrazole–Benzothiadiazole–Pyrazole Photosensitizer into Metal–Organic Frameworks for Photocatalytic Aerobic Oxidation.pdf</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>_cleaned_Building a Pyrazole–Benzothiadiazole–Pyrazole Photosensitizer into Metal–Organic Frameworks for Photocatalytic Aerobic Oxidation.pdf</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>_cleaned_Cancer Cell-Targeted Photosensitizer and Therapeutic Protein Co-Delivery Nanoplatform Based on a Metal-Organic Framework for Enhanced Synergistic Photodynamic and Protein Therapy.pdf</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>_cleaned_Cancer in nonagenarians_ Profile, treatments and outcomes.pdf</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>_cleaned_Cascade Reactions Catalyzed by Planar Metal–Organic Framework Hybrid Architecture for Combined Cancer Therapy.pdf</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>_cleaned_Chemodynamic and Photothermal Combination Therapy Based on Dual-Modified Metal-Organic Framework for Inducing Tumor Ferroptosis_Pyroptosis.pdf</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>_cleaned_Combining Ruthenium(II) Complexes with Metal-Organic Frameworks to Realize Effective Two-Photon Absorption for Singlet Oxygen Generation.pdf</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>_cleaned_Conductivity, doping, and redox chemistry of a microporous dithiolene-based metal-organic framework.pdf</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>_cleaned_Building a Pyrazole–Benzothiadiazole–Pyrazole Photosensitizer into Metal–Organic Frameworks for Photocatalytic Aerobic Oxidation.pdf</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>_cleaned_Cancer Cell-Targeted Photosensitizer and Therapeutic Protein Co-Delivery Nanoplatform Based on a Metal-Organic Framework for Enhanced Synergistic Photodynamic and Protein Therapy.pdf</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>_cleaned_Cancer in nonagenarians_ Profile, treatments and outcomes.pdf</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>_cleaned_Cascade Reactions Catalyzed by Planar Metal–Organic Framework Hybrid Architecture for Combined Cancer Therapy.pdf</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>No valid OCR output</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>